<commit_message>
to check that graphs will change
</commit_message>
<xml_diff>
--- a/exports/movies_report.xlsx
+++ b/exports/movies_report.xlsx
@@ -12,9 +12,9 @@
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="ratings_trend" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'top_movies'!$A$1:$F$11</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'top_movies'!$A$1:$E$11</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'genres_stats'!$A$1:$D$21</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'ratings_trend'!$A$1:$C$25</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'ratings_trend'!$A$1:$C$26</definedName>
   </definedNames>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
@@ -449,7 +449,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F11"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -471,20 +471,15 @@
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>total_ratings</t>
+          <t>avg_rating</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>avg_rating</t>
+          <t>rating_count</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>top_genome_tags</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>short_title</t>
         </is>
@@ -492,266 +487,216 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>318</v>
+        <v>90464</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Shawshank Redemption, The (1994)</t>
+          <t>Frozen North, The (2006)</t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>97999</v>
+        <v>4.8</v>
       </c>
       <c r="D2" t="n">
-        <v>4.42</v>
+        <v>5</v>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>imdb top 250, oscar (best picture), masterpiece, prison, powerful ending</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>Shawshank Redemption, The (1994)</t>
+          <t>Frozen North, The (2006)</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>356</v>
+        <v>185669</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Forrest Gump (1994)</t>
+          <t>CM Punk: Best in the World (2012)</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>97040</v>
+        <v>4.7</v>
       </c>
       <c r="D3" t="n">
-        <v>4.06</v>
+        <v>5</v>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>oscar (best music - original score), oscar (best effects - visual effects), oscar (best picture), oscar (best editing), destiny</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>Forrest Gump (1994)</t>
+          <t>CM Punk: Best in the World (2012)</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>296</v>
+        <v>150228</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Pulp Fiction (1994)</t>
+          <t>Inner Worlds, Outer Worlds (2012)</t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>92406</v>
+        <v>4.6</v>
       </c>
       <c r="D4" t="n">
-        <v>4.17</v>
+        <v>5</v>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>hit men, gratuitous violence, dark humor, masterpiece, storytelling</t>
-        </is>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>Pulp Fiction (1994)</t>
+          <t>Inner Worlds, Outer Worlds (2012)</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>593</v>
+        <v>176113</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Silence of the Lambs, The (1991)</t>
+          <t>Can't Buy My Love (2017)</t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>87899</v>
+        <v>4.6</v>
       </c>
       <c r="D5" t="n">
-        <v>4.15</v>
+        <v>5</v>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>serial killer, oscar (best directing), suspenseful, psychological, psychology</t>
-        </is>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>Silence of the Lambs, The (1991)</t>
+          <t>Can't Buy My Love (2017)</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>2571</v>
+        <v>171705</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Matrix, The (1999)</t>
+          <t>Den radio (2001)</t>
         </is>
       </c>
       <c r="C6" t="n">
-        <v>84545</v>
+        <v>4.58</v>
       </c>
       <c r="D6" t="n">
-        <v>4.15</v>
+        <v>13</v>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>dystopic future, scifi, cyberpunk, science fiction, sci fi</t>
-        </is>
-      </c>
-      <c r="F6" t="inlineStr">
-        <is>
-          <t>Matrix, The (1999)</t>
+          <t>Den radio (2001)</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>260</v>
+        <v>104119</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Star Wars: Episode IV - A New Hope (1977)</t>
+          <t>Forsyte Saga, The (1967)</t>
         </is>
       </c>
       <c r="C7" t="n">
-        <v>81815</v>
+        <v>4.5</v>
       </c>
       <c r="D7" t="n">
-        <v>4.12</v>
+        <v>6</v>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>space opera, trilogy, science fiction, scifi, sci fi</t>
-        </is>
-      </c>
-      <c r="F7" t="inlineStr">
-        <is>
-          <t>Star Wars: Episode IV - A New Hope (1977)</t>
+          <t>Forsyte Saga, The (1967)</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>480</v>
+        <v>173309</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Jurassic Park (1993)</t>
+          <t>Legend of the Galactic Heroes: Overture to a New War (1993)</t>
         </is>
       </c>
       <c r="C8" t="n">
-        <v>76451</v>
+        <v>4.5</v>
       </c>
       <c r="D8" t="n">
-        <v>3.67</v>
+        <v>6</v>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>special effects, dinosaurs, spielberg, big budget, adventure</t>
-        </is>
-      </c>
-      <c r="F8" t="inlineStr">
-        <is>
-          <t>Jurassic Park (1993)</t>
+          <t>Legend of the Galactic Heroes: Overture to a New War (1993)</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>527</v>
+        <v>139096</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Schindler's List (1993)</t>
+          <t>Unmatched (2010)</t>
         </is>
       </c>
       <c r="C9" t="n">
-        <v>71516</v>
+        <v>4.5</v>
       </c>
       <c r="D9" t="n">
-        <v>4.26</v>
+        <v>5</v>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>jews, holocaust, oscar (best directing), nazis, world war ii</t>
-        </is>
-      </c>
-      <c r="F9" t="inlineStr">
-        <is>
-          <t>Schindler's List (1993)</t>
+          <t>Unmatched (2010)</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>110</v>
+        <v>91007</v>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Braveheart (1995)</t>
+          <t>I Want to Be a Soldier (2011)</t>
         </is>
       </c>
       <c r="C10" t="n">
-        <v>68803</v>
+        <v>4.5</v>
       </c>
       <c r="D10" t="n">
-        <v>4.01</v>
+        <v>5</v>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>historical, history, oscar (best directing), oscar (best picture), epic</t>
-        </is>
-      </c>
-      <c r="F10" t="inlineStr">
-        <is>
-          <t>Braveheart (1995)</t>
+          <t>I Want to Be a Soldier (2011)</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>1</v>
+        <v>176569</v>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Toy Story (1995)</t>
+          <t>Liberation Day (2016)</t>
         </is>
       </c>
       <c r="C11" t="n">
-        <v>68469</v>
+        <v>4.5</v>
       </c>
       <c r="D11" t="n">
-        <v>3.89</v>
+        <v>5</v>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>toys, computer animation, pixar animation, animation, kids and family</t>
-        </is>
-      </c>
-      <c r="F11" t="inlineStr">
-        <is>
-          <t>Toy Story (1995)</t>
+          <t>Liberation Day (2016)</t>
         </is>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:F11"/>
+  <autoFilter ref="A1:E11"/>
   <conditionalFormatting sqref="A2:A11">
     <cfRule type="colorScale" priority="1">
       <colorScale>
@@ -1233,7 +1178,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C25"/>
+  <dimension ref="A1:C26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -1523,9 +1468,20 @@
         <v>33660</v>
       </c>
     </row>
+    <row r="26">
+      <c r="A26" t="n">
+        <v>2025</v>
+      </c>
+      <c r="B26" t="n">
+        <v>3</v>
+      </c>
+      <c r="C26" t="n">
+        <v>2</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:C25"/>
-  <conditionalFormatting sqref="A2:A25">
+  <autoFilter ref="A1:C26"/>
+  <conditionalFormatting sqref="A2:A26">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>
@@ -1537,13 +1493,13 @@
       </colorScale>
     </cfRule>
     <cfRule type="expression" priority="2" dxfId="0">
-      <formula>=A2=MAX($A$2:$A$25)</formula>
+      <formula>=A2=MAX($A$2:$A$26)</formula>
     </cfRule>
     <cfRule type="expression" priority="3" dxfId="1">
-      <formula>=A2=MIN($A$2:$A$25)</formula>
+      <formula>=A2=MIN($A$2:$A$26)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B2:B25">
+  <conditionalFormatting sqref="B2:B26">
     <cfRule type="colorScale" priority="4">
       <colorScale>
         <cfvo type="min"/>
@@ -1555,13 +1511,13 @@
       </colorScale>
     </cfRule>
     <cfRule type="expression" priority="5" dxfId="0">
-      <formula>=B2=MAX($B$2:$B$25)</formula>
+      <formula>=B2=MAX($B$2:$B$26)</formula>
     </cfRule>
     <cfRule type="expression" priority="6" dxfId="1">
-      <formula>=B2=MIN($B$2:$B$25)</formula>
+      <formula>=B2=MIN($B$2:$B$26)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C2:C25">
+  <conditionalFormatting sqref="C2:C26">
     <cfRule type="colorScale" priority="7">
       <colorScale>
         <cfvo type="min"/>
@@ -1573,10 +1529,10 @@
       </colorScale>
     </cfRule>
     <cfRule type="expression" priority="8" dxfId="0">
-      <formula>=C2=MAX($C$2:$C$25)</formula>
+      <formula>=C2=MAX($C$2:$C$26)</formula>
     </cfRule>
     <cfRule type="expression" priority="9" dxfId="1">
-      <formula>=C2=MIN($C$2:$C$25)</formula>
+      <formula>=C2=MIN($C$2:$C$26)</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>